<commit_message>
Se adiciona archivo del Modelo, se actualiza BD y se adiciona archivo codigos Ciiu
</commit_message>
<xml_diff>
--- a/BD/Codigos Ciiu.xlsx
+++ b/BD/Codigos Ciiu.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandra Jimenez\Documents\ANALISIS_DE_DATOS_KEY_CODE\Proyecto Final\BD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandra Jimenez\Documents\ANALISIS_DE_DATOS_KEY_CODE\ProyectoFinal\proyecto-final-analisis-datos\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828E54AD-081F-480E-B63A-DA582A25A6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572F6EAF-8DF9-44A2-851D-81EAC8271251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{73F351D0-1FB0-4DBA-913C-7E6BC265B804}"/>
   </bookViews>
@@ -1250,12 +1250,6 @@
     <t>Actividades de organizaciones y entidades extraterritoriales</t>
   </si>
   <si>
-    <t>Otra</t>
-  </si>
-  <si>
-    <t>s clasificaciones</t>
-  </si>
-  <si>
     <t>Asalariados</t>
   </si>
   <si>
@@ -1560,6 +1554,12 @@
   </si>
   <si>
     <t>Actividades no diferenciadas de los hogares individuales como productores de servicios para uso propio</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> clasificaciones</t>
+  </si>
+  <si>
+    <t>Otras</t>
   </si>
 </sst>
 </file>
@@ -1691,35 +1691,6 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1777,13 +1748,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1796,6 +1760,42 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1814,11 +1814,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EC631A8B-7C4C-4E45-8E23-509D987F96DA}" name="Tabla1" displayName="Tabla1" ref="A1:B506" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EC631A8B-7C4C-4E45-8E23-509D987F96DA}" name="Tabla1" displayName="Tabla1" ref="A1:B506" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <autoFilter ref="A1:B506" xr:uid="{EC631A8B-7C4C-4E45-8E23-509D987F96DA}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{8CC8D916-79DC-42C5-B3CC-389BA0622917}" name="Código " dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{E9DE28C5-71B6-4D88-ACC4-39C63CA6F07A}" name="Actividad" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{8CC8D916-79DC-42C5-B3CC-389BA0622917}" name="Código " dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{E9DE28C5-71B6-4D88-ACC4-39C63CA6F07A}" name="Actividad" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2143,8 +2143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BC3F43-415D-43E5-A461-C1AAF821B47D}">
   <dimension ref="A1:B506"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A489" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A501" sqref="A501"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2155,10 +2155,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
@@ -2177,7 +2177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>113</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>122</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>123</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>124</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>128</v>
       </c>
@@ -2281,15 +2281,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>130</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>141</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>142</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>143</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>144</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>145</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>149</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>150</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>161</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>162</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>163</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>164</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>170</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>210</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>220</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>230</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>240</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>311</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>312</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>321</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>322</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>510</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>520</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>610</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>620</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>710</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>721</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>722</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>723</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>729</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>811</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>812</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>820</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>891</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>892</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>899</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>910</v>
       </c>
@@ -2577,15 +2577,15 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>990</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>1011</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>1012</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>1020</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>1030</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>1040</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>1051</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>1052</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>1061</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>1062</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>1063</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>1071</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>1072</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>1081</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>1082</v>
       </c>
@@ -2697,15 +2697,15 @@
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>1083</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>1084</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>1089</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>1090</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>1101</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>1102</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>1103</v>
       </c>
@@ -2753,15 +2753,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="126.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>1104</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>1200</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>1311</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>1312</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>1313</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>1391</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>1392</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>1393</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>1394</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>1399</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>1410</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>1420</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>1430</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>1511</v>
       </c>
@@ -2865,23 +2865,23 @@
         <v>83</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="184" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>1512</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="161" x14ac:dyDescent="0.35">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>1513</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>1521</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>1522</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>1523</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>1610</v>
       </c>
@@ -2913,23 +2913,23 @@
         <v>87</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="161" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>1620</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>1630</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>1640</v>
       </c>
@@ -2937,15 +2937,15 @@
         <v>88</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="115" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>1690</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>1701</v>
       </c>
@@ -2953,15 +2953,15 @@
         <v>89</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="138" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>1702</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>1709</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>1811</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>1812</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>1820</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>1910</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>1921</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>1922</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>2011</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>2012</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>2013</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>2014</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>2021</v>
       </c>
@@ -3057,23 +3057,23 @@
         <v>101</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>2022</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="115" x14ac:dyDescent="0.35">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>2023</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>2029</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>2030</v>
       </c>
@@ -3089,15 +3089,15 @@
         <v>103</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="126.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>2100</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>2211</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>2212</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>2219</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>2221</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>2229</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>2310</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>2391</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
         <v>2392</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>2393</v>
       </c>
@@ -3169,7 +3169,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>2394</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
         <v>2395</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>2396</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
         <v>2399</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
         <v>2410</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
         <v>2421</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
         <v>2429</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
         <v>2431</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
         <v>2432</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
         <v>2511</v>
       </c>
@@ -3249,23 +3249,23 @@
         <v>122</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="138" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
         <v>2512</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" ht="126.5" x14ac:dyDescent="0.35">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
         <v>2513</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
         <v>2520</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
         <v>2591</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
         <v>2592</v>
       </c>
@@ -3289,15 +3289,15 @@
         <v>125</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
         <v>2593</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
         <v>2599</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
         <v>2610</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
         <v>2620</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
         <v>2630</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
         <v>2640</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
         <v>2651</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" s="1">
         <v>2652</v>
       </c>
@@ -3353,15 +3353,15 @@
         <v>132</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" s="1">
         <v>2660</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" s="1">
         <v>2670</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" s="1">
         <v>2680</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" s="1">
         <v>2711</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" s="1">
         <v>2712</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" s="1">
         <v>2720</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
         <v>2731</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
         <v>2732</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
         <v>2740</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
         <v>2750</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
         <v>2790</v>
       </c>
@@ -3441,15 +3441,15 @@
         <v>142</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
         <v>2811</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
         <v>2812</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
         <v>2813</v>
       </c>
@@ -3465,15 +3465,15 @@
         <v>144</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
         <v>2814</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" s="1">
         <v>2815</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
         <v>2816</v>
       </c>
@@ -3489,15 +3489,15 @@
         <v>146</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="115" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" s="1">
         <v>2817</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" s="1">
         <v>2818</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" s="1">
         <v>2819</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" s="1">
         <v>2821</v>
       </c>
@@ -3521,7 +3521,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" s="1">
         <v>2822</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" s="1">
         <v>2823</v>
       </c>
@@ -3537,31 +3537,31 @@
         <v>151</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="115" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" s="1">
         <v>2824</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" s="1">
         <v>2825</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" ht="126.5" x14ac:dyDescent="0.35">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" s="1">
         <v>2826</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" s="1">
         <v>2829</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" s="1">
         <v>2910</v>
       </c>
@@ -3577,23 +3577,23 @@
         <v>153</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="138" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" s="1">
         <v>2920</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" s="1">
         <v>2930</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" s="1">
         <v>3011</v>
       </c>
@@ -3601,7 +3601,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" s="1">
         <v>3012</v>
       </c>
@@ -3609,7 +3609,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" s="1">
         <v>3020</v>
       </c>
@@ -3617,7 +3617,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" s="1">
         <v>3030</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" s="1">
         <v>3040</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" s="1">
         <v>3091</v>
       </c>
@@ -3641,15 +3641,15 @@
         <v>159</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" s="1">
         <v>3092</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" s="1">
         <v>3099</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" s="1">
         <v>3110</v>
       </c>
@@ -3665,7 +3665,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" s="1">
         <v>3120</v>
       </c>
@@ -3673,7 +3673,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" s="1">
         <v>3210</v>
       </c>
@@ -3681,7 +3681,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" s="1">
         <v>3220</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" s="1">
         <v>3230</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" s="1">
         <v>3240</v>
       </c>
@@ -3705,15 +3705,15 @@
         <v>166</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="115" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" s="1">
         <v>3250</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" s="1">
         <v>3290</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" s="1">
         <v>3311</v>
       </c>
@@ -3729,7 +3729,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" s="1">
         <v>3312</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" s="1">
         <v>3313</v>
       </c>
@@ -3745,7 +3745,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" s="1">
         <v>3314</v>
       </c>
@@ -3753,23 +3753,23 @@
         <v>171</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="138" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" s="1">
         <v>3315</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" s="1">
         <v>3319</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" s="1">
         <v>3320</v>
       </c>
@@ -3777,7 +3777,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" s="1">
         <v>3511</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="205" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" s="1">
         <v>3512</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" s="1">
         <v>3513</v>
       </c>
@@ -3801,7 +3801,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="207" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" s="1">
         <v>3514</v>
       </c>
@@ -3809,7 +3809,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" s="1">
         <v>3520</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" s="1">
         <v>3530</v>
       </c>
@@ -3825,7 +3825,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="210" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" s="1">
         <v>3600</v>
       </c>
@@ -3833,7 +3833,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="211" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" s="1">
         <v>3700</v>
       </c>
@@ -3841,7 +3841,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="212" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" s="1">
         <v>3811</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="213" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" s="1">
         <v>3812</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" s="1">
         <v>3821</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" s="1">
         <v>3822</v>
       </c>
@@ -3873,7 +3873,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="216" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" s="1">
         <v>3830</v>
       </c>
@@ -3881,15 +3881,15 @@
         <v>185</v>
       </c>
     </row>
-    <row r="217" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" s="1">
         <v>3900</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" s="1">
         <v>4111</v>
       </c>
@@ -3897,7 +3897,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="219" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" s="1">
         <v>4112</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="220" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" s="1">
         <v>4210</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="221" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" s="1">
         <v>4220</v>
       </c>
@@ -3921,7 +3921,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="222" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" s="1">
         <v>4290</v>
       </c>
@@ -3929,7 +3929,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="223" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" s="1">
         <v>4311</v>
       </c>
@@ -3937,7 +3937,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="224" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" s="1">
         <v>4312</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="225" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" s="1">
         <v>4321</v>
       </c>
@@ -3953,7 +3953,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="226" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" s="1">
         <v>4322</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="227" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" s="1">
         <v>4329</v>
       </c>
@@ -3969,7 +3969,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="228" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" s="1">
         <v>4330</v>
       </c>
@@ -3977,15 +3977,15 @@
         <v>196</v>
       </c>
     </row>
-    <row r="229" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" s="1">
         <v>4390</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" s="1">
         <v>4511</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="231" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" s="1">
         <v>4512</v>
       </c>
@@ -4001,7 +4001,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="232" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" s="1">
         <v>4520</v>
       </c>
@@ -4009,15 +4009,15 @@
         <v>199</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" s="1">
         <v>4530</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" s="1">
         <v>4541</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" s="1">
         <v>4542</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" s="1">
         <v>4610</v>
       </c>
@@ -4041,7 +4041,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="237" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" s="1">
         <v>4620</v>
       </c>
@@ -4049,7 +4049,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="238" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" s="1">
         <v>4631</v>
       </c>
@@ -4057,7 +4057,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" s="1">
         <v>4632</v>
       </c>
@@ -4065,15 +4065,15 @@
         <v>205</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" s="1">
         <v>4641</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" s="1">
         <v>4642</v>
       </c>
@@ -4081,7 +4081,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" s="1">
         <v>4643</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" s="1">
         <v>4644</v>
       </c>
@@ -4097,15 +4097,15 @@
         <v>208</v>
       </c>
     </row>
-    <row r="244" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" s="1">
         <v>4645</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" s="1">
         <v>4649</v>
       </c>
@@ -4113,23 +4113,23 @@
         <v>209</v>
       </c>
     </row>
-    <row r="246" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" s="1">
         <v>4651</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" ht="115" x14ac:dyDescent="0.35">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" s="1">
         <v>4652</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" s="1">
         <v>4653</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="249" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" s="1">
         <v>4659</v>
       </c>
@@ -4145,15 +4145,15 @@
         <v>211</v>
       </c>
     </row>
-    <row r="250" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250" s="1">
         <v>4661</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251" s="1">
         <v>4662</v>
       </c>
@@ -4161,23 +4161,23 @@
         <v>212</v>
       </c>
     </row>
-    <row r="252" spans="1:2" ht="149.5" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" s="1">
         <v>4663</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" ht="161" x14ac:dyDescent="0.35">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A253" s="1">
         <v>4664</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254" s="1">
         <v>4665</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="255" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A255" s="1">
         <v>4669</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="256" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A256" s="1">
         <v>4690</v>
       </c>
@@ -4201,63 +4201,63 @@
         <v>215</v>
       </c>
     </row>
-    <row r="257" spans="1:2" ht="149.5" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257" s="1">
         <v>4711</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" ht="195.5" x14ac:dyDescent="0.35">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A258" s="1">
         <v>4719</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" ht="126.5" x14ac:dyDescent="0.35">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A259" s="1">
         <v>4721</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" ht="126.5" x14ac:dyDescent="0.35">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260" s="1">
         <v>4722</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" ht="172.5" x14ac:dyDescent="0.35">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261" s="1">
         <v>4723</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" ht="115" x14ac:dyDescent="0.35">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A262" s="1">
         <v>4724</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" ht="126.5" x14ac:dyDescent="0.35">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A263" s="1">
         <v>4729</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A264" s="1">
         <v>4731</v>
       </c>
@@ -4265,63 +4265,63 @@
         <v>216</v>
       </c>
     </row>
-    <row r="265" spans="1:2" ht="126.5" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A265" s="1">
         <v>4732</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" ht="172.5" x14ac:dyDescent="0.35">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A266" s="1">
         <v>4741</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" ht="126.5" x14ac:dyDescent="0.35">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A267" s="1">
         <v>4742</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A268" s="1">
         <v>4751</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" ht="138" x14ac:dyDescent="0.35">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A269" s="1">
         <v>4752</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" ht="138" x14ac:dyDescent="0.35">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A270" s="1">
         <v>4753</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" ht="126.5" x14ac:dyDescent="0.35">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A271" s="1">
         <v>4754</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A272" s="1">
         <v>4755</v>
       </c>
@@ -4329,71 +4329,71 @@
         <v>217</v>
       </c>
     </row>
-    <row r="273" spans="1:2" ht="126.5" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A273" s="1">
         <v>4759</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" ht="149.5" x14ac:dyDescent="0.35">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A274" s="1">
         <v>4761</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" ht="115" x14ac:dyDescent="0.35">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A275" s="1">
         <v>4762</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" ht="149.5" x14ac:dyDescent="0.35">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A276" s="1">
         <v>4769</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" ht="149.5" x14ac:dyDescent="0.35">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A277" s="1">
         <v>4771</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2" ht="149.5" x14ac:dyDescent="0.35">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A278" s="1">
         <v>4772</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" ht="161" x14ac:dyDescent="0.35">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A279" s="1">
         <v>4773</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" ht="115" x14ac:dyDescent="0.35">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A280" s="1">
         <v>4774</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A281" s="1">
         <v>4775</v>
       </c>
@@ -4401,23 +4401,23 @@
         <v>218</v>
       </c>
     </row>
-    <row r="282" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A282" s="1">
         <v>4781</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2" ht="115" x14ac:dyDescent="0.35">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A283" s="1">
         <v>4782</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A284" s="1">
         <v>4789</v>
       </c>
@@ -4425,7 +4425,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="285" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A285" s="1">
         <v>4791</v>
       </c>
@@ -4433,7 +4433,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="286" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A286" s="1">
         <v>4792</v>
       </c>
@@ -4441,15 +4441,15 @@
         <v>221</v>
       </c>
     </row>
-    <row r="287" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A287" s="1">
         <v>4799</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A288" s="1">
         <v>4911</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="289" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A289" s="1">
         <v>4912</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="290" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A290" s="1">
         <v>4921</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="291" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A291" s="1">
         <v>4922</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="292" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A292" s="1">
         <v>4923</v>
       </c>
@@ -4489,7 +4489,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="293" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A293" s="1">
         <v>4930</v>
       </c>
@@ -4497,7 +4497,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="294" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A294" s="1">
         <v>5011</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="295" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A295" s="1">
         <v>5012</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="296" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A296" s="1">
         <v>5021</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="297" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A297" s="1">
         <v>5022</v>
       </c>
@@ -4529,7 +4529,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="298" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A298" s="1">
         <v>5111</v>
       </c>
@@ -4537,7 +4537,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="299" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A299" s="1">
         <v>5112</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="300" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A300" s="1">
         <v>5121</v>
       </c>
@@ -4553,7 +4553,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="301" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A301" s="1">
         <v>5122</v>
       </c>
@@ -4561,7 +4561,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="302" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A302" s="1">
         <v>5210</v>
       </c>
@@ -4569,31 +4569,31 @@
         <v>236</v>
       </c>
     </row>
-    <row r="303" spans="1:2" ht="115" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A303" s="1">
         <v>5221</v>
       </c>
       <c r="B303" s="2" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A304" s="1">
         <v>5222</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="305" spans="1:2" ht="138" x14ac:dyDescent="0.35">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A305" s="1">
         <v>5223</v>
       </c>
       <c r="B305" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="306" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A306" s="1">
         <v>5224</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="307" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A307" s="1">
         <v>5229</v>
       </c>
@@ -4609,7 +4609,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="308" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A308" s="1">
         <v>5310</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="309" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A309" s="1">
         <v>5320</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="310" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A310" s="1">
         <v>5511</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="311" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A311" s="1">
         <v>5512</v>
       </c>
@@ -4641,7 +4641,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="312" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A312" s="1">
         <v>5513</v>
       </c>
@@ -4649,7 +4649,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="313" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A313" s="1">
         <v>5514</v>
       </c>
@@ -4657,7 +4657,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="314" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A314" s="1">
         <v>5519</v>
       </c>
@@ -4665,7 +4665,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="315" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A315" s="1">
         <v>5520</v>
       </c>
@@ -4673,7 +4673,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="316" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A316" s="1">
         <v>5530</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="317" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A317" s="1">
         <v>5590</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="318" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A318" s="1">
         <v>5611</v>
       </c>
@@ -4697,7 +4697,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="319" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A319" s="1">
         <v>5612</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="320" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A320" s="1">
         <v>5613</v>
       </c>
@@ -4713,7 +4713,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="321" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A321" s="1">
         <v>5619</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="322" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A322" s="1">
         <v>5621</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="323" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A323" s="1">
         <v>5629</v>
       </c>
@@ -4737,7 +4737,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="324" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A324" s="1">
         <v>5630</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="325" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A325" s="1">
         <v>5811</v>
       </c>
@@ -4753,7 +4753,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="326" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A326" s="1">
         <v>5812</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="327" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A327" s="1">
         <v>5813</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="328" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A328" s="1">
         <v>5819</v>
       </c>
@@ -4777,7 +4777,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="329" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A329" s="1">
         <v>5820</v>
       </c>
@@ -4785,31 +4785,31 @@
         <v>260</v>
       </c>
     </row>
-    <row r="330" spans="1:2" ht="126.5" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A330" s="1">
         <v>5911</v>
       </c>
       <c r="B330" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="331" spans="1:2" ht="126.5" x14ac:dyDescent="0.35">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A331" s="1">
         <v>5912</v>
       </c>
       <c r="B331" s="2" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="332" spans="1:2" ht="126.5" x14ac:dyDescent="0.35">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A332" s="1">
         <v>5913</v>
       </c>
       <c r="B332" s="2" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="333" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A333" s="1">
         <v>5914</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="334" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A334" s="1">
         <v>5920</v>
       </c>
@@ -4825,15 +4825,15 @@
         <v>262</v>
       </c>
     </row>
-    <row r="335" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A335" s="1">
         <v>6010</v>
       </c>
       <c r="B335" s="2" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="336" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A336" s="1">
         <v>6020</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="337" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A337" s="1">
         <v>6110</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="338" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A338" s="1">
         <v>6120</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="339" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A339" s="1">
         <v>6130</v>
       </c>
@@ -4865,7 +4865,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="340" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A340" s="1">
         <v>6190</v>
       </c>
@@ -4873,31 +4873,31 @@
         <v>267</v>
       </c>
     </row>
-    <row r="341" spans="1:2" ht="115" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A341" s="1">
         <v>6201</v>
       </c>
       <c r="B341" s="2" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="342" spans="1:2" ht="126.5" x14ac:dyDescent="0.35">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A342" s="1">
         <v>6202</v>
       </c>
       <c r="B342" s="2" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="343" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A343" s="1">
         <v>6209</v>
       </c>
       <c r="B343" s="2" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="344" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A344" s="1">
         <v>6311</v>
       </c>
@@ -4905,7 +4905,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="345" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A345" s="1">
         <v>6312</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="346" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A346" s="1">
         <v>6391</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="347" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A347" s="1">
         <v>6399</v>
       </c>
@@ -4929,7 +4929,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="348" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A348" s="1">
         <v>6411</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="349" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A349" s="1">
         <v>6412</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="350" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A350" s="1">
         <v>6421</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="351" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A351" s="1">
         <v>6422</v>
       </c>
@@ -4961,7 +4961,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="352" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A352" s="1">
         <v>6423</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="353" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A353" s="1">
         <v>6424</v>
       </c>
@@ -4977,7 +4977,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="354" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A354" s="1">
         <v>6431</v>
       </c>
@@ -4985,7 +4985,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="355" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A355" s="1">
         <v>6432</v>
       </c>
@@ -4993,7 +4993,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="356" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A356" s="1">
         <v>6491</v>
       </c>
@@ -5001,15 +5001,15 @@
         <v>280</v>
       </c>
     </row>
-    <row r="357" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A357" s="1">
         <v>6492</v>
       </c>
       <c r="B357" s="2" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="358" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A358" s="1">
         <v>6493</v>
       </c>
@@ -5017,7 +5017,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="359" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A359" s="1">
         <v>6494</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="360" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A360" s="1">
         <v>6495</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="361" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A361" s="1">
         <v>6496</v>
       </c>
@@ -5041,15 +5041,15 @@
         <v>284</v>
       </c>
     </row>
-    <row r="362" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A362" s="1">
         <v>6499</v>
       </c>
       <c r="B362" s="2" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="363" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A363" s="1">
         <v>6511</v>
       </c>
@@ -5057,7 +5057,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="364" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A364" s="1">
         <v>6512</v>
       </c>
@@ -5065,7 +5065,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="365" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A365" s="1">
         <v>6513</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="366" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A366" s="1">
         <v>6515</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="367" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A367" s="1">
         <v>6521</v>
       </c>
@@ -5089,7 +5089,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="368" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A368" s="1">
         <v>6522</v>
       </c>
@@ -5097,7 +5097,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="369" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A369" s="1">
         <v>6523</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="370" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A370" s="1">
         <v>6531</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="371" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A371" s="1">
         <v>6532</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="372" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A372" s="1">
         <v>6611</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="373" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A373" s="1">
         <v>6612</v>
       </c>
@@ -5137,7 +5137,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="374" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A374" s="1">
         <v>6613</v>
       </c>
@@ -5145,7 +5145,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="375" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A375" s="1">
         <v>6614</v>
       </c>
@@ -5153,7 +5153,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="376" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A376" s="1">
         <v>6615</v>
       </c>
@@ -5161,15 +5161,15 @@
         <v>298</v>
       </c>
     </row>
-    <row r="377" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A377" s="1">
         <v>6619</v>
       </c>
       <c r="B377" s="2" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="378" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A378" s="1">
         <v>6621</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="379" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A379" s="1">
         <v>6629</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="380" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A380" s="1">
         <v>6630</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="381" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A381" s="1">
         <v>6810</v>
       </c>
@@ -5201,15 +5201,15 @@
         <v>302</v>
       </c>
     </row>
-    <row r="382" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" s="1">
         <v>6820</v>
       </c>
       <c r="B382" s="2" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="383" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A383" s="1">
         <v>6910</v>
       </c>
@@ -5217,15 +5217,15 @@
         <v>303</v>
       </c>
     </row>
-    <row r="384" spans="1:2" ht="115" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A384" s="1">
         <v>6920</v>
       </c>
       <c r="B384" s="2" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="385" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A385" s="1">
         <v>7010</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="386" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A386" s="1">
         <v>7020</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="387" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A387" s="1">
         <v>7111</v>
       </c>
@@ -5249,15 +5249,15 @@
         <v>306</v>
       </c>
     </row>
-    <row r="388" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A388" s="1">
         <v>7112</v>
       </c>
       <c r="B388" s="2" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="389" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A389" s="1">
         <v>7120</v>
       </c>
@@ -5265,23 +5265,23 @@
         <v>307</v>
       </c>
     </row>
-    <row r="390" spans="1:2" ht="115" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A390" s="1">
         <v>7210</v>
       </c>
       <c r="B390" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="391" spans="1:2" ht="115" x14ac:dyDescent="0.35">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A391" s="1">
         <v>7220</v>
       </c>
       <c r="B391" s="2" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="392" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A392" s="1">
         <v>7310</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="393" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A393" s="1">
         <v>7320</v>
       </c>
@@ -5297,7 +5297,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="394" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A394" s="1">
         <v>7410</v>
       </c>
@@ -5305,7 +5305,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="395" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A395" s="1">
         <v>7420</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="396" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A396" s="1">
         <v>7490</v>
       </c>
@@ -5321,7 +5321,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="397" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A397" s="1">
         <v>7500</v>
       </c>
@@ -5329,7 +5329,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="398" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A398" s="1">
         <v>7710</v>
       </c>
@@ -5337,7 +5337,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="399" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A399" s="1">
         <v>7721</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="400" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A400" s="1">
         <v>7722</v>
       </c>
@@ -5353,31 +5353,31 @@
         <v>316</v>
       </c>
     </row>
-    <row r="401" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A401" s="1">
         <v>7729</v>
       </c>
       <c r="B401" s="2" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="402" spans="1:2" ht="115" x14ac:dyDescent="0.35">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A402" s="1">
         <v>7730</v>
       </c>
       <c r="B402" s="2" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="403" spans="1:2" ht="138" x14ac:dyDescent="0.35">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A403" s="1">
         <v>7740</v>
       </c>
       <c r="B403" s="2" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="404" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A404" s="1">
         <v>7810</v>
       </c>
@@ -5385,7 +5385,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="405" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A405" s="1">
         <v>7820</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="406" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A406" s="1">
         <v>7830</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="407" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A407" s="1">
         <v>7911</v>
       </c>
@@ -5409,7 +5409,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="408" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A408" s="1">
         <v>7912</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="409" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A409" s="1">
         <v>7990</v>
       </c>
@@ -5425,7 +5425,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="410" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A410" s="1">
         <v>8010</v>
       </c>
@@ -5433,7 +5433,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="411" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A411" s="1">
         <v>8020</v>
       </c>
@@ -5441,7 +5441,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="412" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A412" s="1">
         <v>8030</v>
       </c>
@@ -5449,7 +5449,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="413" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A413" s="1">
         <v>8110</v>
       </c>
@@ -5457,7 +5457,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="414" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A414" s="1">
         <v>8121</v>
       </c>
@@ -5465,7 +5465,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="415" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A415" s="1">
         <v>8129</v>
       </c>
@@ -5473,7 +5473,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="416" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A416" s="1">
         <v>8130</v>
       </c>
@@ -5481,7 +5481,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="417" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A417" s="1">
         <v>8211</v>
       </c>
@@ -5489,15 +5489,15 @@
         <v>330</v>
       </c>
     </row>
-    <row r="418" spans="1:2" ht="115" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A418" s="1">
         <v>8219</v>
       </c>
       <c r="B418" s="2" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="419" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A419" s="1">
         <v>8220</v>
       </c>
@@ -5505,7 +5505,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="420" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="420" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A420" s="1">
         <v>8230</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="421" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="421" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A421" s="1">
         <v>8291</v>
       </c>
@@ -5521,7 +5521,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="422" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="422" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A422" s="1">
         <v>8292</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="423" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="423" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A423" s="1">
         <v>8299</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="424" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A424" s="1">
         <v>8411</v>
       </c>
@@ -5545,7 +5545,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="425" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A425" s="1">
         <v>8412</v>
       </c>
@@ -5553,15 +5553,15 @@
         <v>337</v>
       </c>
     </row>
-    <row r="426" spans="1:2" ht="207" x14ac:dyDescent="0.35">
+    <row r="426" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A426" s="1">
         <v>8413</v>
       </c>
       <c r="B426" s="2" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="427" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A427" s="1">
         <v>8414</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="428" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="428" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A428" s="1">
         <v>8415</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="429" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="429" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A429" s="1">
         <v>8421</v>
       </c>
@@ -5585,7 +5585,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="430" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="430" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A430" s="1">
         <v>8422</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="431" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="431" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A431" s="1">
         <v>8423</v>
       </c>
@@ -5601,7 +5601,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="432" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="432" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A432" s="1">
         <v>8424</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="433" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="433" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A433" s="1">
         <v>8430</v>
       </c>
@@ -5617,7 +5617,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="434" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="434" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A434" s="1">
         <v>8511</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="435" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="435" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A435" s="1">
         <v>8512</v>
       </c>
@@ -5633,7 +5633,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="436" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="436" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A436" s="1">
         <v>8513</v>
       </c>
@@ -5641,7 +5641,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="437" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="437" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A437" s="1">
         <v>8521</v>
       </c>
@@ -5649,7 +5649,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="438" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="438" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A438" s="1">
         <v>8522</v>
       </c>
@@ -5657,7 +5657,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="439" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="439" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A439" s="1">
         <v>8523</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="440" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="440" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A440" s="1">
         <v>8530</v>
       </c>
@@ -5673,7 +5673,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="441" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="441" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A441" s="1">
         <v>8541</v>
       </c>
@@ -5681,7 +5681,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="442" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="442" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A442" s="1">
         <v>8542</v>
       </c>
@@ -5689,7 +5689,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="443" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="443" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A443" s="1">
         <v>8543</v>
       </c>
@@ -5697,7 +5697,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="444" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="444" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A444" s="1">
         <v>8544</v>
       </c>
@@ -5705,7 +5705,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="445" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="445" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A445" s="1">
         <v>8551</v>
       </c>
@@ -5713,7 +5713,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="446" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="446" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A446" s="1">
         <v>8552</v>
       </c>
@@ -5721,7 +5721,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="447" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="447" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A447" s="1">
         <v>8553</v>
       </c>
@@ -5729,7 +5729,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="448" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="448" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A448" s="1">
         <v>8559</v>
       </c>
@@ -5737,7 +5737,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="449" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="449" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A449" s="1">
         <v>8560</v>
       </c>
@@ -5745,7 +5745,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="450" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="450" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A450" s="1">
         <v>8610</v>
       </c>
@@ -5753,7 +5753,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="451" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="451" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A451" s="1">
         <v>8621</v>
       </c>
@@ -5761,7 +5761,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="452" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="452" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A452" s="1">
         <v>8622</v>
       </c>
@@ -5769,7 +5769,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="453" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="453" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A453" s="1">
         <v>8691</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="454" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="454" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A454" s="1">
         <v>8692</v>
       </c>
@@ -5785,7 +5785,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="455" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="455" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A455" s="1">
         <v>8699</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="456" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="456" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A456" s="1">
         <v>8710</v>
       </c>
@@ -5801,23 +5801,23 @@
         <v>367</v>
       </c>
     </row>
-    <row r="457" spans="1:2" ht="161" x14ac:dyDescent="0.35">
+    <row r="457" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A457" s="1">
         <v>8720</v>
       </c>
       <c r="B457" s="2" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="458" spans="1:2" ht="126.5" x14ac:dyDescent="0.35">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A458" s="1">
         <v>8730</v>
       </c>
       <c r="B458" s="2" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="459" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A459" s="1">
         <v>8790</v>
       </c>
@@ -5825,15 +5825,15 @@
         <v>368</v>
       </c>
     </row>
-    <row r="460" spans="1:2" ht="115" x14ac:dyDescent="0.35">
+    <row r="460" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A460" s="1">
         <v>8810</v>
       </c>
       <c r="B460" s="2" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="461" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A461" s="1">
         <v>8891</v>
       </c>
@@ -5841,7 +5841,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="462" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="462" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A462" s="1">
         <v>8899</v>
       </c>
@@ -5849,7 +5849,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="463" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="463" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A463" s="1">
         <v>9001</v>
       </c>
@@ -5857,7 +5857,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="464" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="464" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A464" s="1">
         <v>9002</v>
       </c>
@@ -5865,7 +5865,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="465" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="465" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A465" s="1">
         <v>9003</v>
       </c>
@@ -5873,7 +5873,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="466" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="466" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A466" s="1">
         <v>9004</v>
       </c>
@@ -5881,7 +5881,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="467" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="467" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A467" s="1">
         <v>9005</v>
       </c>
@@ -5889,7 +5889,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="468" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="468" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A468" s="1">
         <v>9006</v>
       </c>
@@ -5897,7 +5897,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="469" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="469" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A469" s="1">
         <v>9007</v>
       </c>
@@ -5905,7 +5905,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="470" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="470" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A470" s="1">
         <v>9008</v>
       </c>
@@ -5913,7 +5913,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="471" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="471" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A471" s="1">
         <v>9101</v>
       </c>
@@ -5921,15 +5921,15 @@
         <v>379</v>
       </c>
     </row>
-    <row r="472" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="472" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A472" s="1">
         <v>9102</v>
       </c>
       <c r="B472" s="2" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="473" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A473" s="1">
         <v>9103</v>
       </c>
@@ -5937,7 +5937,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="474" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="474" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A474" s="1">
         <v>9200</v>
       </c>
@@ -5945,7 +5945,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="475" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="475" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A475" s="1">
         <v>9311</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="476" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="476" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A476" s="1">
         <v>9312</v>
       </c>
@@ -5961,7 +5961,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="477" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="477" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A477" s="1">
         <v>9319</v>
       </c>
@@ -5969,7 +5969,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="478" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="478" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A478" s="1">
         <v>9321</v>
       </c>
@@ -5977,7 +5977,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="479" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="479" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A479" s="1">
         <v>9329</v>
       </c>
@@ -5985,7 +5985,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="480" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="480" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A480" s="1">
         <v>9411</v>
       </c>
@@ -5993,7 +5993,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="481" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="481" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A481" s="1">
         <v>9412</v>
       </c>
@@ -6001,7 +6001,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="482" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="482" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A482" s="1">
         <v>9420</v>
       </c>
@@ -6009,7 +6009,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="483" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="483" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A483" s="1">
         <v>9491</v>
       </c>
@@ -6017,7 +6017,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="484" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="484" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A484" s="1">
         <v>9492</v>
       </c>
@@ -6025,7 +6025,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="485" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="485" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A485" s="1">
         <v>9499</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="486" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="486" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A486" s="1">
         <v>9511</v>
       </c>
@@ -6041,7 +6041,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="487" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+    <row r="487" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A487" s="1">
         <v>9512</v>
       </c>
@@ -6049,7 +6049,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="488" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="488" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A488" s="1">
         <v>9521</v>
       </c>
@@ -6057,7 +6057,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="489" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="489" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A489" s="1">
         <v>9522</v>
       </c>
@@ -6065,7 +6065,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="490" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="490" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A490" s="1">
         <v>9523</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="491" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="491" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A491" s="1">
         <v>9524</v>
       </c>
@@ -6081,7 +6081,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="492" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="492" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A492" s="1">
         <v>9529</v>
       </c>
@@ -6089,15 +6089,15 @@
         <v>399</v>
       </c>
     </row>
-    <row r="493" spans="1:2" ht="92" x14ac:dyDescent="0.35">
+    <row r="493" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A493" s="1">
         <v>9601</v>
       </c>
       <c r="B493" s="2" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="494" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="494" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A494" s="1">
         <v>9602</v>
       </c>
@@ -6105,7 +6105,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="495" spans="1:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="495" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A495" s="1">
         <v>9603</v>
       </c>
@@ -6113,7 +6113,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="496" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="496" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A496" s="1">
         <v>9609</v>
       </c>
@@ -6121,31 +6121,31 @@
         <v>402</v>
       </c>
     </row>
-    <row r="497" spans="1:2" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="497" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A497" s="1">
         <v>9700</v>
       </c>
       <c r="B497" s="2" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="498" spans="1:2" ht="138" x14ac:dyDescent="0.35">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="498" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A498" s="1">
         <v>9810</v>
       </c>
       <c r="B498" s="2" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="499" spans="1:2" ht="138" x14ac:dyDescent="0.35">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="499" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A499" s="1">
         <v>9820</v>
       </c>
       <c r="B499" s="2" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="500" spans="1:2" ht="80.5" x14ac:dyDescent="0.35">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="500" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A500" s="1">
         <v>9900</v>
       </c>
@@ -6153,52 +6153,52 @@
         <v>403</v>
       </c>
     </row>
-    <row r="501" spans="1:2" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="501" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A501" s="1" t="s">
-        <v>404</v>
+        <v>507</v>
       </c>
       <c r="B501" s="2" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="502" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="502" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A502" s="1">
         <v>10</v>
       </c>
       <c r="B502" s="2" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="503" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="503" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A503" s="1">
         <v>20</v>
       </c>
       <c r="B503" s="2" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="504" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="504" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A504" s="1">
         <v>81</v>
       </c>
       <c r="B504" s="2" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="505" spans="1:2" ht="57.5" x14ac:dyDescent="0.35">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="505" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A505" s="1">
         <v>82</v>
       </c>
       <c r="B505" s="2" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="506" spans="1:2" ht="69" x14ac:dyDescent="0.35">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="506" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A506" s="5">
         <v>90</v>
       </c>
       <c r="B506" s="6" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>